<commit_message>
V0.5.0 Updated blogs and home. Some additional information about the application context
</commit_message>
<xml_diff>
--- a/example-springboot/src/main/resources/static/content.xlsx
+++ b/example-springboot/src/main/resources/static/content.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/werner.diwischek/dev/elasticobjects/example-springboot/src/main/resources/static/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E68EEDC2-74CA-D147-9C79-E2292840EE9A}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0B015148-553B-0144-9D1F-28D3D465AB5D}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="280" yWindow="460" windowWidth="28240" windowHeight="17100" activeTab="1" xr2:uid="{046F7480-149E-4041-B8FC-50A00BC9D93F}"/>
+    <workbookView xWindow="560" yWindow="7260" windowWidth="28240" windowHeight="17100" activeTab="2" xr2:uid="{046F7480-149E-4041-B8FC-50A00BC9D93F}"/>
   </bookViews>
   <sheets>
     <sheet name="intro" sheetId="1" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="73" uniqueCount="70">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="74" uniqueCount="71">
   <si>
     <t>head</t>
   </si>
@@ -285,9 +285,6 @@
 &lt;textarea&gt;EO eoRoot = new EoRoot(cache, anObject);&lt;/textarea&gt;&lt;textarea&gt;eoRoot.set(otherObject, "aPath");&lt;/textarea&gt;</t>
   </si>
   <si>
-    <t>Why a bean call is better than a remote method calls?</t>
-  </si>
-  <si>
     <t xml:space="preserve">Is it a solution where you can defer the framework solution? </t>
   </si>
   <si>
@@ -345,6 +342,12 @@
 access&lt;/li&gt;&lt;li&gt;&lt;a href="/configs/DbSqlConfig.html"&gt;DbSqlConfig.json&lt;/a&gt; for database access&lt;/li&gt;&lt;/ul&gt;
 A configured call has a configuration key within, where the configuration is connected. The configuration implements some methods to access a file, a list or execute some sql.
 These configuration extends ConfigResources class, which contains some role access definitions.</t>
+  </si>
+  <si>
+    <t>Why a bean call is better than a remote method call?</t>
+  </si>
+  <si>
+    <t>https://www.sueddeutsche.de/wissen/kuenstliche-intelligenz-software-computer-1.5036926?utm_source=pocket-newtab-global-de-DE</t>
   </si>
 </sst>
 </file>
@@ -1100,8 +1103,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B990D812-5E7E-114D-98B5-934CEA6081DB}">
   <dimension ref="A1:C11"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" zoomScale="118" workbookViewId="0">
-      <selection activeCell="B7" sqref="B7"/>
+    <sheetView topLeftCell="A9" zoomScale="118" workbookViewId="0">
+      <selection activeCell="B10" sqref="B10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1151,7 +1154,7 @@
         <v>51</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="C4" s="1" t="str">
         <f t="shared" si="0"/>
@@ -1163,7 +1166,7 @@
         <v>57</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="C5" s="1" t="str">
         <f t="shared" si="0"/>
@@ -1175,7 +1178,7 @@
         <v>52</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="C6" s="1" t="str">
         <f t="shared" si="0"/>
@@ -1187,7 +1190,7 @@
         <v>53</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="C7" s="1" t="str">
         <f t="shared" si="0"/>
@@ -1199,7 +1202,7 @@
         <v>54</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="C8" s="1" t="str">
         <f t="shared" si="0"/>
@@ -1211,7 +1214,7 @@
         <v>55</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="C9" s="1" t="str">
         <f>CONCATENATE("FAQ: ",A9)</f>
@@ -1220,22 +1223,22 @@
     </row>
     <row r="10" spans="1:3" ht="136" x14ac:dyDescent="0.2">
       <c r="A10" s="1" t="s">
-        <v>60</v>
+        <v>69</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="C10" s="1" t="str">
         <f>CONCATENATE("FAQ: ",A10)</f>
-        <v>FAQ: Why a bean call is better than a remote method calls?</v>
+        <v>FAQ: Why a bean call is better than a remote method call?</v>
       </c>
     </row>
     <row r="11" spans="1:3" ht="204" x14ac:dyDescent="0.2">
       <c r="A11" s="1" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="C11" s="1" t="str">
         <f>CONCATENATE("FAQ: ",A11)</f>
@@ -1249,9 +1252,11 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BC7CDFA3-6D82-E245-B11F-41EF1E8C10A5}">
-  <dimension ref="A1:C12"/>
+  <dimension ref="A1:C13"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A13" sqref="A13"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
@@ -1321,6 +1326,11 @@
         <v>49</v>
       </c>
     </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A13" t="s">
+        <v>70</v>
+      </c>
+    </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="A11" r:id="rId1" xr:uid="{63EAACCC-2DF9-E643-86D4-BB1405E6FE42}"/>

</xml_diff>